<commit_message>
edited harp lake rain files
</commit_message>
<xml_diff>
--- a/HarpLake/HarpRain.xlsx
+++ b/HarpLake/HarpRain.xlsx
@@ -376,8 +376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4019"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4019"/>
+    <sheetView tabSelected="1" topLeftCell="A3941" workbookViewId="0">
+      <selection activeCell="B3956" sqref="A2:B4019"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10430,7 +10430,7 @@
         <v>34493</v>
       </c>
       <c r="B1256" s="3">
-        <v>-0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1257" spans="1:2" x14ac:dyDescent="0.3">
@@ -19782,7 +19782,7 @@
         <v>35662</v>
       </c>
       <c r="B2425" s="3">
-        <v>-0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2426" spans="1:2" x14ac:dyDescent="0.3">
@@ -20558,7 +20558,7 @@
         <v>35759</v>
       </c>
       <c r="B2522" s="3">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2523" spans="1:2" x14ac:dyDescent="0.3">
@@ -32190,7 +32190,7 @@
         <v>37213</v>
       </c>
       <c r="B3976" s="3">
-        <v>-7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3977" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>